<commit_message>
Refactored phip-seq Ig normalization
</commit_message>
<xml_diff>
--- a/psot/ELISA-robot-template.xlsx
+++ b/psot/ELISA-robot-template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16440" yWindow="11000" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="2020" yWindow="1120" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ELISA-robot-template" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>sample_id</t>
   </si>
@@ -35,35 +35,311 @@
     <t>source_well</t>
   </si>
   <si>
-    <t>conc_plate1</t>
-  </si>
-  <si>
-    <t>conc_plate2</t>
-  </si>
-  <si>
-    <t>additional_columns_allowed</t>
-  </si>
-  <si>
-    <t>always_µg_per_mL</t>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>A9</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>A11</t>
+  </si>
+  <si>
+    <t>A12</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>B8</t>
+  </si>
+  <si>
+    <t>B9</t>
+  </si>
+  <si>
+    <t>B10</t>
+  </si>
+  <si>
+    <t>B11</t>
+  </si>
+  <si>
+    <t>B12</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>D11</t>
+  </si>
+  <si>
+    <t>D12</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>E7</t>
+  </si>
+  <si>
+    <t>E8</t>
+  </si>
+  <si>
+    <t>E9</t>
+  </si>
+  <si>
+    <t>E10</t>
+  </si>
+  <si>
+    <t>E11</t>
+  </si>
+  <si>
+    <t>E12</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t>F6</t>
+  </si>
+  <si>
+    <t>F7</t>
+  </si>
+  <si>
+    <t>F8</t>
+  </si>
+  <si>
+    <t>F9</t>
+  </si>
+  <si>
+    <t>F10</t>
+  </si>
+  <si>
+    <t>F11</t>
+  </si>
+  <si>
+    <t>F12</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>G3</t>
+  </si>
+  <si>
+    <t>G4</t>
+  </si>
+  <si>
+    <t>G5</t>
+  </si>
+  <si>
+    <t>G6</t>
+  </si>
+  <si>
+    <t>G7</t>
+  </si>
+  <si>
+    <t>G8</t>
+  </si>
+  <si>
+    <t>G9</t>
+  </si>
+  <si>
+    <t>G10</t>
+  </si>
+  <si>
+    <t>G11</t>
+  </si>
+  <si>
+    <t>G12</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>H4</t>
+  </si>
+  <si>
+    <t>H5</t>
+  </si>
+  <si>
+    <t>H6</t>
+  </si>
+  <si>
+    <t>H7</t>
+  </si>
+  <si>
+    <t>H8</t>
+  </si>
+  <si>
+    <t>H9</t>
+  </si>
+  <si>
+    <t>H10</t>
+  </si>
+  <si>
+    <t>H11</t>
+  </si>
+  <si>
+    <t>H12</t>
+  </si>
+  <si>
+    <t>conc_plate_1_ug_ml</t>
+  </si>
+  <si>
+    <t>conc_plate_2_ug_ml</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -86,9 +362,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -98,6 +373,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -366,15 +644,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:D97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -382,47 +665,491 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="1"/>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B66" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B67" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B69" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B70" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B71" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B72" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B73" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B74" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B75" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B76" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B77" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B78" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B79" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B80" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B81" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B82" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B83" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B84" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B85" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B86" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B87" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B88" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B89" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B90" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B91" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B92" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B93" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B94" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B95" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B96" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B97" t="s">
+        <v>97</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Refactored for more flexible input file
</commit_message>
<xml_diff>
--- a/psot/ELISA-robot-template.xlsx
+++ b/psot/ELISA-robot-template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laserson/repos/robots/psot/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF58D9C-3707-FB4C-BD72-5F9A2492CAFB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2020" yWindow="1120" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="1040" windowWidth="28160" windowHeight="16880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ELISA-robot-template" sheetId="1" r:id="rId1"/>
@@ -29,9 +30,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
-    <t>sample_id</t>
-  </si>
-  <si>
     <t>source_well</t>
   </si>
   <si>
@@ -327,12 +325,15 @@
   </si>
   <si>
     <t>conc_plate_2_ug_ml</t>
+  </si>
+  <si>
+    <t>library_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -643,11 +644,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -659,496 +660,496 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" t="s">
         <v>98</v>
-      </c>
-      <c r="D1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added add'l useful cols to psot template
</commit_message>
<xml_diff>
--- a/psot/ELISA-robot-template.xlsx
+++ b/psot/ELISA-robot-template.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laserson/repos/robots/psot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF58D9C-3707-FB4C-BD72-5F9A2492CAFB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32874B93-7174-F340-B9A6-C02FD520161B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1040" windowWidth="28160" windowHeight="16880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5940" yWindow="3620" windowWidth="19120" windowHeight="13020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ELISA-robot-template" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
   <si>
     <t>source_well</t>
   </si>
@@ -328,6 +328,21 @@
   </si>
   <si>
     <t>library_id</t>
+  </si>
+  <si>
+    <t>sample_id</t>
+  </si>
+  <si>
+    <t>project</t>
+  </si>
+  <si>
+    <t>bc_well</t>
+  </si>
+  <si>
+    <t>bc_seq</t>
+  </si>
+  <si>
+    <t>bc_read</t>
   </si>
 </sst>
 </file>
@@ -645,510 +660,527 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D97"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>99</v>
       </c>
       <c r="B1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>97</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+      <c r="G1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
+    <row r="32" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B37" t="s">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B39" t="s">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D43" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B44" t="s">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D44" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B45" t="s">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D45" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D46" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B47" t="s">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D47" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B48" t="s">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D48" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B49" t="s">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D49" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B50" t="s">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D50" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B51" t="s">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B52" t="s">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B53" t="s">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D53" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B54" t="s">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D54" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B55" t="s">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D55" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B56" t="s">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D56" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B57" t="s">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D57" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B58" t="s">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D58" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B59" t="s">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D59" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B60" t="s">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D60" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B61" t="s">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D61" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B62" t="s">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D62" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B63" t="s">
+    <row r="63" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D63" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B64" t="s">
+    <row r="64" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D64" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B65" t="s">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D65" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B66" t="s">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D66" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B67" t="s">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D67" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B68" t="s">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D68" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B69" t="s">
+    <row r="69" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D69" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B70" t="s">
+    <row r="70" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D70" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B71" t="s">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D71" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B72" t="s">
+    <row r="72" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D72" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B73" t="s">
+    <row r="73" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D73" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B74" t="s">
+    <row r="74" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D74" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B75" t="s">
+    <row r="75" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D75" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B76" t="s">
+    <row r="76" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D76" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B77" t="s">
+    <row r="77" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D77" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B78" t="s">
+    <row r="78" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D78" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B79" t="s">
+    <row r="79" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D79" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B80" t="s">
+    <row r="80" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D80" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B81" t="s">
+    <row r="81" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D81" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B82" t="s">
+    <row r="82" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D82" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B83" t="s">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D83" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B84" t="s">
+    <row r="84" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D84" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B85" t="s">
+    <row r="85" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D85" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B86" t="s">
+    <row r="86" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D86" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B87" t="s">
+    <row r="87" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D87" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B88" t="s">
+    <row r="88" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D88" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B89" t="s">
+    <row r="89" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D89" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B90" t="s">
+    <row r="90" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D90" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B91" t="s">
+    <row r="91" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D91" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B92" t="s">
+    <row r="92" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D92" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B93" t="s">
+    <row r="93" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D93" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B94" t="s">
+    <row r="94" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D94" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B95" t="s">
+    <row r="95" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D95" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B96" t="s">
+    <row r="96" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D96" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B97" t="s">
+    <row r="97" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D97" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>